<commit_message>
Ajout fichier de remise
</commit_message>
<xml_diff>
--- a/Remises/Répartition des tâches.xlsx
+++ b/Remises/Répartition des tâches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dodo-\source\repos\Exercices_ITV\TP3\Remises\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A5ABC55-F63F-4B8A-99D9-A9252CAEC676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E18C3FA-4BE5-457E-A4EA-DDF03F871BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AC3522B6-DB6A-4E9F-8C3B-7BEBDA643225}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Nom</t>
   </si>
@@ -50,48 +50,16 @@
     <t>Jean-Philippe Delisle</t>
   </si>
   <si>
-    <t>Les pipelines doivent se déclencher automatiquement à chaque modification des branches "main" et "develop"</t>
-  </si>
-  <si>
     <t>Étape 3 - Remise</t>
   </si>
   <si>
     <t>Vidéo sur YouTube</t>
   </si>
   <si>
-    <t>Étape 1 - Gestion de source et intégration continue</t>
-  </si>
-  <si>
-    <t>Copies d'écran</t>
-  </si>
-  <si>
     <t>Répartition des tâches entre partenaires avec nombre d'heures</t>
   </si>
   <si>
     <t>Répondre aux questions suivantes</t>
-  </si>
-  <si>
-    <r>
-      <t>Ajoutez </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF24292F"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>pfleon@csfoy.ca</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF24292F"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t> comme utilisateur et administrateur</t>
-    </r>
   </si>
   <si>
     <r>
@@ -117,55 +85,25 @@
     </r>
   </si>
   <si>
-    <t>Créer un groupe de ressource</t>
-  </si>
-  <si>
-    <t>Créer une base de données SQL</t>
-  </si>
-  <si>
-    <t>Créer un site web</t>
-  </si>
-  <si>
-    <t>Créer un pipeline classic d'intégration continue qui construit 4 artefacts</t>
-  </si>
-  <si>
-    <t>Créer un nouveau projet d'équipe et y ajouter le code du projet</t>
-  </si>
-  <si>
-    <t>Créer une branche "develop"</t>
-  </si>
-  <si>
-    <t>Étape 2 - Création des ressources Azure</t>
-  </si>
-  <si>
-    <t>Étape 3 - Déploiement continu</t>
-  </si>
-  <si>
-    <t>Manuel d'utilisation de votre pipeline d'intégration continue </t>
-  </si>
-  <si>
-    <t>Exporter fichier ARM</t>
-  </si>
-  <si>
-    <t>Créer un release pipeline Dévelopment - Stage Unitaire</t>
-  </si>
-  <si>
-    <t>Créer un release pipeline Dévelopment - Stage Fonctionnel</t>
-  </si>
-  <si>
-    <t>Créer les Variables des releases pipelines</t>
-  </si>
-  <si>
-    <t>Créer une release pipeline Production - Stage Unitaire</t>
-  </si>
-  <si>
-    <t>Créer une release pipeline Production - Stage Production</t>
-  </si>
-  <si>
-    <t>Créer une release pipeline Production - Stage Fonctionnel</t>
-  </si>
-  <si>
-    <t>Valider les déploiements dans Azure</t>
+    <t>Étape 1 - Création d'un fichier Dockerfile</t>
+  </si>
+  <si>
+    <t>Étape 2 - Création des fichiers YAML de déploiement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total (heure) : </t>
+  </si>
+  <si>
+    <t>Création du fichier Dockerfile</t>
+  </si>
+  <si>
+    <t>Créer repos DockerHub et validation</t>
+  </si>
+  <si>
+    <t>Créer le fichier YAML</t>
+  </si>
+  <si>
+    <t>Créer le script Powershell</t>
   </si>
 </sst>
 </file>
@@ -583,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1225EC97-B17E-426D-A013-3E2D86F5999E}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -616,209 +554,143 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="5" t="str">
-        <f>SUM(B4:B7)&amp;"h"</f>
-        <v>0h</v>
-      </c>
-      <c r="C3" s="5" t="str">
-        <f>SUM(C4:C7)&amp;"h"</f>
-        <v>0h</v>
+        <v>9</v>
+      </c>
+      <c r="B3" s="5">
+        <f>SUM(B4:B5)</f>
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="5">
+        <f>SUM(C4:C5)</f>
+        <v>3.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="5">
+        <f>SUM(B7:B8)</f>
+        <v>17</v>
+      </c>
+      <c r="C6" s="5">
+        <f>SUM(C7:C8)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="7">
+        <v>14</v>
+      </c>
+      <c r="C7" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="7">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="5">
-        <f>SUM(B9:B12)</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="5">
-        <f>SUM(C9:C12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="5">
+        <f>SUM(B10:B13)</f>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="C9" s="5">
+        <f>SUM(C10:C13)</f>
+        <v>2.2000000000000002</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="B10" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="7">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+        <v>6</v>
+      </c>
+      <c r="B11" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="5">
-        <f>SUM(B14:B20)</f>
+        <v>7</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="C12" s="7">
         <v>0</v>
       </c>
-      <c r="C13" s="5">
-        <f>SUM(C14:C20)</f>
-        <v>0</v>
+    </row>
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0.1</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-    </row>
-    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-    </row>
-    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="5">
-        <f>SUM(B22:B28)</f>
-        <v>0</v>
-      </c>
-      <c r="C21" s="5">
-        <f>SUM(C22:C28)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-    </row>
-    <row r="23" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-    </row>
-    <row r="24" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-    </row>
-    <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A25" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-    </row>
-    <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-    </row>
-    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="B14">
+        <f>SUM(B9+B6+B3)</f>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="C14">
+        <f>SUM(C9+C6+C3)</f>
+        <v>16.7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -826,6 +698,6 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>